<commit_message>
End-to-end process type testing
</commit_message>
<xml_diff>
--- a/testcase/books-api-test-cases-final.xlsx
+++ b/testcase/books-api-test-cases-final.xlsx
@@ -498,9 +498,6 @@
     <t>Book removed successfully.</t>
   </si>
   <si>
-    <t>@api @functional @e2e @flow</t>
-  </si>
-  <si>
     <t>B024</t>
   </si>
   <si>
@@ -517,6 +514,9 @@
   </si>
   <si>
     <t>Query fails with appropriate error.</t>
+  </si>
+  <si>
+    <t>@api @functional @e2e @flow</t>
   </si>
   <si>
     <t>B025</t>
@@ -546,7 +546,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,13 +556,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1032,148 +1025,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2356,12 +2349,12 @@
         <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -2373,25 +2366,25 @@
         <v>14</v>
       </c>
       <c r="E25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" t="s">
         <v>150</v>
-      </c>
-      <c r="F25" t="s">
-        <v>151</v>
       </c>
       <c r="G25" t="s">
         <v>139</v>
       </c>
       <c r="H25" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" t="s">
         <v>152</v>
-      </c>
-      <c r="I25" t="s">
-        <v>153</v>
       </c>
       <c r="J25" t="s">
         <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2426,7 +2419,7 @@
         <v>20</v>
       </c>
       <c r="K26" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>